<commit_message>
updated users and user sports
</commit_message>
<xml_diff>
--- a/database/seeds/user_sports.xlsx
+++ b/database/seeds/user_sports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/glenn/Documents/NUS/Hackers/eusoff/database/seeds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{884BD3B4-53A0-584D-9AC7-B26286665BBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F32326-88BC-B54C-A93F-B11CF58EE223}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5580" yWindow="2360" windowWidth="27640" windowHeight="16940" xr2:uid="{9FC50BC8-1DAF-3A43-8B40-45CEFA48CE84}"/>
   </bookViews>
@@ -399,9 +399,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{025A19F7-2308-D741-91F4-25365B430BF3}">
-  <dimension ref="A1:C729"/>
+  <dimension ref="A1:C730"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A715" workbookViewId="0">
+      <selection activeCell="C730" sqref="C730"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6345,7 +6347,7 @@
         <v>308</v>
       </c>
       <c r="C540" s="1">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="541" spans="1:3" x14ac:dyDescent="0.2">
@@ -8425,6 +8427,17 @@
       </c>
       <c r="C729" s="1">
         <v>7</v>
+      </c>
+    </row>
+    <row r="730" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A730" s="1">
+        <v>729</v>
+      </c>
+      <c r="B730" s="1">
+        <v>67</v>
+      </c>
+      <c r="C730" s="1">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>